<commit_message>
feat: Implementación de envío de correos y visualización de datos
- Agregado sistema de envío de correos con PDF de resultados
- Implementada generación de gráficos interactivos
- Actualizado .gitignore y dependencias
- Añadidos nuevos archivos de utilidades y formularios
- Actualizadas plantillas y estilos
</commit_message>
<xml_diff>
--- a/DESCRIPTORES_EVALUACION_GESTION_RIESGO.xlsx
+++ b/DESCRIPTORES_EVALUACION_GESTION_RIESGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://crcsa-my.sharepoint.com/personal/analista1_grd_crantioquia_org_co/Documents/Documentos/DOCUMENTOS CONSTRUIDOS DE BASE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRUZ_ROJA\Scripts\Matriz_Madurez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69FB1014-FE39-45D5-AFCF-993D2281BE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE482C37-AAF3-497B-B37C-5F5889365AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A225F0FC-ACD1-41BB-89D4-9094B3759ACB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A225F0FC-ACD1-41BB-89D4-9094B3759ACB}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptores" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Descriptores!$B$1:$J$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Descriptores!$B$1:$L$38</definedName>
     <definedName name="Type">'[1]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -441,9 +441,6 @@
     <t>EQ1</t>
   </si>
   <si>
-    <t>Control de acceso</t>
-  </si>
-  <si>
     <t>No existe controles de acceso a los lugares o recursos de la organización</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
     <t>Todas las areas llevan a cabo retroalimentacion de sus actividades organizacionales y estas, son tomadas en cuenta para la mejora de los procesos</t>
   </si>
   <si>
-    <t>IT6</t>
-  </si>
-  <si>
     <t>Mecanismos de articulación interinstitucional</t>
   </si>
   <si>
@@ -672,9 +666,6 @@
     <t>Los mecanismos de articulacion interinstiucional se definen para cada actividad, proyecto u obra en gestion del riesgo y emergencias.</t>
   </si>
   <si>
-    <t>ORGANIZACIÓN</t>
-  </si>
-  <si>
     <t>OR1</t>
   </si>
   <si>
@@ -778,6 +769,15 @@
   </si>
   <si>
     <t>Existe una politica de diversidad e inclusion adoptada en el la organizaicion y se utiliza para dar soporte a las decisiones</t>
+  </si>
+  <si>
+    <t>Control de acceso a instalaciones</t>
+  </si>
+  <si>
+    <t>IT4</t>
+  </si>
+  <si>
+    <t>ORGANIZACIÓN Y ESTRUCTURA</t>
   </si>
 </sst>
 </file>
@@ -869,7 +869,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -892,128 +892,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1022,55 +908,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,1176 +1310,1406 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.375" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="5.875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="29.875" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="30.875" customWidth="1"/>
-    <col min="11" max="11" width="3.375" customWidth="1"/>
-    <col min="12" max="16" width="11" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" customWidth="1"/>
+    <col min="2" max="2" width="20.3984375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="5.8984375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="13" customWidth="1"/>
+    <col min="5" max="6" width="25.5" style="11" customWidth="1"/>
+    <col min="7" max="8" width="24.8984375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="25.5" style="13" customWidth="1"/>
+    <col min="10" max="10" width="29.8984375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="27" style="13" customWidth="1"/>
+    <col min="12" max="12" width="30.8984375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="3.3984375" style="13" customWidth="1"/>
+    <col min="14" max="18" width="11" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="11.09765625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="4">
+        <f>SUM(E3:E10)</f>
+        <v>100</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="10">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12">
+        <v>30</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="H3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="81" x14ac:dyDescent="0.25">
+      <c r="L3" s="21"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="H4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="I4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="J4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="K4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="13" t="s">
+      <c r="L4" s="21"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="H5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="I5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="J5" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="K5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="13" t="s">
+      <c r="L5" s="21"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="10">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="H6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="I6" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="J6" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="K6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="13" t="s">
+      <c r="L6" s="21"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="10">
+        <v>20</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="H7" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="I7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="J7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="K7" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="13" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="H8" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="I8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="J8" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="K8" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="13" t="s">
+      <c r="L8" s="21"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="H9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="I9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="J9" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="K9" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="13" t="s">
+      <c r="L9" s="21"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="10">
+        <v>10</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="H10" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="I10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="J10" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="K10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="12" t="s">
+      <c r="L10" s="21"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10">
+        <f>SUM(E12:E20)</f>
+        <v>100</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E12" s="10">
+        <v>5</v>
+      </c>
+      <c r="F12" s="12">
+        <v>20</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="H12" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="I12" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="J12" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="K12" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="13" t="s">
+      <c r="L12" s="21"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E13" s="10">
+        <v>10</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="H13" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="I13" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="J13" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="K13" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="13" t="s">
+      <c r="L13" s="21"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" customFormat="1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E14" s="10">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="H14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="I14" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="J14" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="K14" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" ht="54" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="13" t="s">
+      <c r="L14" s="21"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D15" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E15" s="10">
+        <v>5</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="H15" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="I15" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="J15" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="K15" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" ht="54" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="13" t="s">
+      <c r="L15" s="21"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D16" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E16" s="10">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="H16" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="I16" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="J16" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="K16" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="13" t="s">
+      <c r="L16" s="21"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D17" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E17" s="10">
+        <v>5</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="H17" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="I17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="J17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="K17" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:16" ht="108" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="13" t="s">
+      <c r="L17" s="21"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D18" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E18" s="10">
+        <v>10</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="H18" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="I18" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="J18" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="K18" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="13" t="s">
+      <c r="L18" s="21"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D19" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E19" s="10">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="H19" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="I19" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="J19" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="K19" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="1:16" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="13" t="s">
+      <c r="L19" s="21"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D20" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E20" s="10">
+        <v>20</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="H20" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="I20" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="J20" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="K20" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="12" t="s">
+      <c r="L20" s="21"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="10">
+        <f>SUM(E22:E27)</f>
+        <v>100</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D22" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E22" s="10">
+        <v>13.4</v>
+      </c>
+      <c r="F22" s="12">
+        <v>30</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="H22" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="I22" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="J22" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="K22" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="L22" s="21"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" customFormat="1" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="1:16" ht="108" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="13" t="s">
+      <c r="D23" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E23" s="10">
+        <v>13.3</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="H23" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="I23" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="J23" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="K23" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="L23" s="21"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="13" t="s">
+      <c r="D24" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E24" s="10">
+        <v>20</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="H24" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="I24" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="J24" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="K24" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="L24" s="21"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="1:18" customFormat="1" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="1:16" ht="189" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="13" t="s">
+      <c r="D25" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="E25" s="10">
+        <v>13.3</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="H25" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="I25" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="J25" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="K25" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="L25" s="21"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" customFormat="1" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="1:16" ht="108" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="13" t="s">
+      <c r="D26" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="E26" s="10">
+        <v>20</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="H26" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="I26" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="J26" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="K26" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="L26" s="21"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="13" t="s">
+      <c r="D27" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="E27" s="10">
+        <v>20</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="H27" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="I27" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="J27" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="K27" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="L27" s="21"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="10">
+        <f>SUM(E29:E33)</f>
+        <v>100</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="1:18" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="J25" s="16"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-    </row>
-    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="1:16" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="20" t="s">
+      <c r="C29" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="D29" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E29" s="10">
+        <v>20</v>
+      </c>
+      <c r="F29" s="12">
+        <v>10</v>
+      </c>
+      <c r="G29" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="H29" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="I29" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="J29" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="K29" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="L29" s="21"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:18" customFormat="1" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="1:16" ht="175.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="13" t="s">
+      <c r="D30" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E30" s="10">
+        <v>25</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="H30" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="I30" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="J30" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="K30" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="L30" s="21"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+    </row>
+    <row r="31" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-    </row>
-    <row r="29" spans="1:16" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="13" t="s">
+      <c r="D31" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E31" s="10">
+        <v>10</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="H31" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="I31" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="J31" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="K31" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="L31" s="21"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="10">
+        <v>25</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="K32" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="L32" s="21"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+    </row>
+    <row r="33" spans="1:18" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="I30" s="16" t="s">
+      <c r="D33" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="13" t="s">
+      <c r="E33" s="10">
+        <v>20</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="H33" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="I33" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="J33" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="K33" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="L33" s="21"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+    </row>
+    <row r="34" spans="1:18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="10">
+        <f>SUM(E35:E39)</f>
+        <v>100</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+    </row>
+    <row r="35" spans="1:18" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="I31" s="16" t="s">
+      <c r="D35" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="20" t="s">
+      <c r="E35" s="10">
+        <v>20</v>
+      </c>
+      <c r="F35" s="12">
+        <v>10</v>
+      </c>
+      <c r="G35" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="H35" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="I35" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="J35" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="K35" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="L35" s="21"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="D36" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="I32" s="16" t="s">
+      <c r="E36" s="10">
+        <v>30</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="J32" s="16"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="13" t="s">
+      <c r="H36" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="I36" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="J36" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="K36" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="L36" s="21"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+    </row>
+    <row r="37" spans="1:18" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="D37" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="I33" s="16" t="s">
+      <c r="E37" s="10">
+        <v>15</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="1:16" ht="54" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="13" t="s">
+      <c r="H37" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="I37" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="J37" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="K37" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="L37" s="21"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="1:18" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="D38" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="E38" s="10">
+        <v>15</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="G38" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:16" ht="81" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="13" t="s">
+      <c r="H38" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="I38" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="J38" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="K38" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="L38" s="21"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="1:18" customFormat="1" ht="132" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="D39" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="I35" s="16" t="s">
+      <c r="E39" s="10">
+        <v>20</v>
+      </c>
+      <c r="F39" s="12"/>
+      <c r="G39" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="J35" s="16"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21" t="s">
+      <c r="H39" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="I39" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="J39" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="F36" s="16" t="s">
+      <c r="K39" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="G36" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="J36" s="22"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-    </row>
-    <row r="38" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+    </row>
+    <row r="41" spans="1:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B1:J1"/>
+  <mergeCells count="12">
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B1:L1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B10"/>
-    <mergeCell ref="B11:B19"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="F12:F20"/>
+    <mergeCell ref="F22:F27"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="F35:F39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0" footer="0"/>

</xml_diff>